<commit_message>
update layout 2 layer
</commit_message>
<xml_diff>
--- a/DE_XUAT_VAT_TU_NGHIEN_CUU_MACH_XA_PIN.xlsx
+++ b/DE_XUAT_VAT_TU_NGHIEN_CUU_MACH_XA_PIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="30690" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>&lt;20 ngày</t>
   </si>
   <si>
-    <t>Mạch in ina_board_2</t>
-  </si>
-  <si>
     <t>Trở 0603 1% 10K (50c)</t>
   </si>
   <si>
@@ -232,17 +229,20 @@
   </si>
   <si>
     <t>https://banlinhkien.com/diode-zener-12w-3.3v-smd1206-zmm3.3-10c-p16720535.html</t>
+  </si>
+  <si>
+    <t>Jump Chốt 2.0MM (10c)</t>
+  </si>
+  <si>
+    <t>https://banlinhkien.com/jump-chot-2.0mm-10c-p18436956.html</t>
   </si>
   <si>
     <t xml:space="preserve">- Căn cứ : ……………………………………………………………………………………………………………
 - Căn cứ: ………………………………………………………………………………………………………
- ( Đơn vị) đề xuất mua sắm…VẬT TƯ PHẦN ĐIỀU KHIỂN BỘ XẢ PIN…...trong tháng……4…………cụ thể như sau: </t>
-  </si>
-  <si>
-    <t>Jump Chốt 2.0MM (10c)</t>
-  </si>
-  <si>
-    <t>https://banlinhkien.com/jump-chot-2.0mm-10c-p18436956.html</t>
+ ( Đơn vị) đề xuất mua sắm…VẬT TƯ PHẦN ĐIỀU KHIỂN BỘ XẢ PIN…...trong tháng……5…………cụ thể như sau: </t>
+  </si>
+  <si>
+    <t>Mạch in pcb</t>
   </si>
 </sst>
 </file>
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +907,7 @@
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -955,11 +955,11 @@
         <v>1</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="10">
         <v>10</v>
@@ -975,7 +975,7 @@
         <v>23</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -983,11 +983,11 @@
         <v>2</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="10">
         <v>10</v>
@@ -1003,7 +1003,7 @@
         <v>23</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,11 +1011,11 @@
         <v>3</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="10">
         <v>10</v>
@@ -1031,7 +1031,7 @@
         <v>23</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1039,11 +1039,11 @@
         <v>4</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="10">
         <v>10</v>
@@ -1059,7 +1059,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1067,11 +1067,11 @@
         <v>5</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="10">
         <v>10</v>
@@ -1087,7 +1087,7 @@
         <v>23</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1095,11 +1095,11 @@
         <v>6</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="10">
         <v>10</v>
@@ -1115,7 +1115,7 @@
         <v>23</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,11 +1123,11 @@
         <v>7</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="10">
         <v>15</v>
@@ -1143,7 +1143,7 @@
         <v>23</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1151,11 +1151,11 @@
         <v>8</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="10">
         <v>100</v>
@@ -1171,7 +1171,7 @@
         <v>23</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1179,11 +1179,11 @@
         <v>9</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="10">
         <v>10</v>
@@ -1199,7 +1199,7 @@
         <v>23</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,11 +1207,11 @@
         <v>10</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="10">
         <v>10</v>
@@ -1227,7 +1227,7 @@
         <v>23</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1235,11 +1235,11 @@
         <v>11</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="10">
         <v>10</v>
@@ -1255,7 +1255,7 @@
         <v>23</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1263,11 +1263,11 @@
         <v>12</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="10">
         <v>20</v>
@@ -1283,7 +1283,7 @@
         <v>23</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
@@ -1311,7 +1311,7 @@
         <v>23</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1319,11 +1319,11 @@
         <v>14</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="10">
         <v>20</v>
@@ -1339,7 +1339,7 @@
         <v>23</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1347,11 +1347,11 @@
         <v>15</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="10">
         <v>20</v>
@@ -1367,7 +1367,7 @@
         <v>23</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
@@ -1395,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,7 +1403,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
@@ -1423,7 +1423,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1431,11 +1431,11 @@
         <v>18</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="10">
         <v>10</v>
@@ -1451,7 +1451,7 @@
         <v>23</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1459,11 +1459,11 @@
         <v>19</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="10">
         <v>15</v>
@@ -1479,7 +1479,7 @@
         <v>23</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10" t="s">

</xml_diff>